<commit_message>
feat: update upload fcl freight, fcl inland, air freight
</commit_message>
<xml_diff>
--- a/src/assets/extra/FclUplaodFormat.xlsx
+++ b/src/assets/extra/FclUplaodFormat.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DREAMWORLD\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A4500B-9D27-4D3F-BBE6-E019434ACB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="FCL" sheetId="1" r:id="rId4"/>
+    <sheet name="FCL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="RwZVHbFxDOgH9Fuann1rof+Uj65Kc6V+2cdeRqDLk/8="/>
@@ -16,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
-  <si>
-    <t>Cargo_type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Cargo_Class</t>
   </si>
@@ -66,9 +72,6 @@
     <t>Destination_Detention_Free</t>
   </si>
   <si>
-    <t>GEN</t>
-  </si>
-  <si>
     <t>INMAA</t>
   </si>
   <si>
@@ -97,32 +100,42 @@
   </si>
   <si>
     <t>IDJKT</t>
+  </si>
+  <si>
+    <t>Cargo_Type</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>Tax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
     </font>
     <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -133,7 +146,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -143,7 +156,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -157,36 +176,40 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -376,333 +399,338 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.56"/>
-    <col customWidth="1" min="2" max="2" width="12.11"/>
-    <col customWidth="1" min="3" max="3" width="8.33"/>
-    <col customWidth="1" min="4" max="13" width="10.56"/>
-    <col customWidth="1" min="14" max="14" width="13.67"/>
-    <col customWidth="1" min="15" max="15" width="23.78"/>
-    <col customWidth="1" min="16" max="16" width="23.56"/>
-    <col customWidth="1" min="17" max="26" width="10.56"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="13" width="10.5" customWidth="1"/>
+    <col min="14" max="14" width="13.625" customWidth="1"/>
+    <col min="15" max="15" width="23.75" customWidth="1"/>
+    <col min="16" max="16" width="23.5" customWidth="1"/>
+    <col min="17" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:17" ht="25.5">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2958</v>
+      </c>
+      <c r="I2" s="3">
+        <v>3958</v>
+      </c>
+      <c r="J2" s="3">
+        <v>3958</v>
+      </c>
+      <c r="N2" s="3">
+        <v>21</v>
+      </c>
+      <c r="O2" s="3">
+        <v>4</v>
+      </c>
+      <c r="P2" s="3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
+    <row r="3" spans="1:17" ht="15.75">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H3" s="3">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3">
+        <v>12</v>
+      </c>
+      <c r="N3" s="3">
+        <v>28</v>
+      </c>
+      <c r="O3" s="3">
+        <v>4</v>
+      </c>
+      <c r="P3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3">
-        <v>2958.0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>3958.0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>3958.0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>21.0</v>
-      </c>
-      <c r="O2" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>4.0</v>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3">
+        <v>12</v>
+      </c>
+      <c r="N4" s="3">
+        <v>27</v>
+      </c>
+      <c r="O4" s="3">
+        <v>4</v>
+      </c>
+      <c r="P4" s="3">
+        <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
+    <row r="5" spans="1:17" ht="15.75">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="H5" s="3">
+        <v>270</v>
+      </c>
+      <c r="I5" s="3">
+        <v>158</v>
+      </c>
+      <c r="J5" s="3">
+        <v>158</v>
+      </c>
+      <c r="N5" s="3">
+        <v>27</v>
+      </c>
+      <c r="O5" s="3">
+        <v>4</v>
+      </c>
+      <c r="P5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="3">
+        <v>270</v>
+      </c>
+      <c r="I6" s="3">
+        <v>158</v>
+      </c>
+      <c r="J6" s="3">
+        <v>158</v>
+      </c>
+      <c r="N6" s="3">
+        <v>27</v>
+      </c>
+      <c r="O6" s="3">
+        <v>4</v>
+      </c>
+      <c r="P6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3">
+        <v>10</v>
+      </c>
+      <c r="I7" s="3">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="J3" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="N3" s="3">
-        <v>28.0</v>
-      </c>
-      <c r="O3" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="P3" s="3">
-        <v>4.0</v>
+      <c r="J7" s="3">
+        <v>20</v>
+      </c>
+      <c r="N7" s="3">
+        <v>27</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4</v>
+      </c>
+      <c r="P7" s="3">
+        <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    <row r="8" spans="1:17" ht="15.75">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>4.0</v>
+      <c r="H8" s="3">
+        <v>105</v>
+      </c>
+      <c r="I8" s="3">
+        <v>70</v>
+      </c>
+      <c r="J8" s="3">
+        <v>70</v>
+      </c>
+      <c r="N8" s="3">
+        <v>27</v>
+      </c>
+      <c r="O8" s="3">
+        <v>4</v>
+      </c>
+      <c r="P8" s="3">
+        <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    <row r="9" spans="1:17" ht="15.75">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="3">
-        <v>270.0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>158.0</v>
-      </c>
-      <c r="J5" s="3">
-        <v>158.0</v>
-      </c>
-      <c r="N5" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="3">
-        <v>270.0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>158.0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>158.0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="3">
-        <v>10.0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="N7" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="O7" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="P7" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="3">
-        <v>105.0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>70.0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>70.0</v>
-      </c>
-      <c r="N8" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="O8" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="P8" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="H9" s="3">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="I9" s="3">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="J9" s="3">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="N9" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="O9" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="P9" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1686,9 +1714,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes related to air and console upload
</commit_message>
<xml_diff>
--- a/src/assets/extra/FclUplaodFormat.xlsx
+++ b/src/assets/extra/FclUplaodFormat.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DREAMWORLD\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myWorkStarted\tarifftales-spa-app\src\assets\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A4500B-9D27-4D3F-BBE6-E019434ACB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1491F8-737D-4114-BA52-6356F60625C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FCL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="RwZVHbFxDOgH9Fuann1rof+Uj65Kc6V+2cdeRqDLk/8="/>
     </ext>
@@ -183,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -409,22 +420,22 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
-    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="2" max="2" width="12.09765625" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" customWidth="1"/>
     <col min="4" max="13" width="10.5" customWidth="1"/>
-    <col min="14" max="14" width="13.625" customWidth="1"/>
-    <col min="15" max="15" width="23.75" customWidth="1"/>
+    <col min="14" max="14" width="13.59765625" customWidth="1"/>
+    <col min="15" max="15" width="23.69921875" customWidth="1"/>
     <col min="16" max="16" width="23.5" customWidth="1"/>
     <col min="17" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.5">
+    <row r="1" spans="1:17" ht="26.4">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -477,7 +488,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75">
+    <row r="2" spans="1:17" ht="15.6">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -509,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75">
+    <row r="3" spans="1:17" ht="15.6">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -541,7 +552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75">
+    <row r="4" spans="1:17" ht="15.6">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -573,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75">
+    <row r="5" spans="1:17" ht="15.6">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -605,7 +616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75">
+    <row r="6" spans="1:17" ht="15.6">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -637,7 +648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75">
+    <row r="7" spans="1:17" ht="15.6">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -669,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75">
+    <row r="8" spans="1:17" ht="15.6">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -701,7 +712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75">
+    <row r="9" spans="1:17" ht="15.6">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1715,6 +1726,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>